<commit_message>
Updated as of 03/03 11am
</commit_message>
<xml_diff>
--- a/12 Chunked Design/Chunked.xlsx
+++ b/12 Chunked Design/Chunked.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tinkertanker/Documents/ESD/40.014 ESA/ESAProject2019Team08/12 Chunked Design/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B18865F-4BE7-8346-9D8C-7B2F3A92E75D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EBF1003-6BC6-7D4F-91E8-0E91B23229CA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="5" xr2:uid="{0FD85137-0B22-4B4D-910E-126022132FD4}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="164">
   <si>
     <t>Generic Player (one of several)</t>
   </si>
@@ -508,6 +508,27 @@
   </si>
   <si>
     <t>Collect User Survey</t>
+  </si>
+  <si>
+    <t>Player</t>
+  </si>
+  <si>
+    <t>Tile type System</t>
+  </si>
+  <si>
+    <t>Map Progress System</t>
+  </si>
+  <si>
+    <t>Card Interaction System</t>
+  </si>
+  <si>
+    <t>Progress Tracking System</t>
+  </si>
+  <si>
+    <t>Deck Management System</t>
+  </si>
+  <si>
+    <t>Reset Game to Initial Status</t>
   </si>
 </sst>
 </file>
@@ -1826,7 +1847,7 @@
   <dimension ref="B1:E59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
@@ -1837,16 +1858,16 @@
   <sheetData>
     <row r="1" spans="2:5" ht="16">
       <c r="B1" s="6" t="s">
-        <v>0</v>
+        <v>157</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>1</v>
+        <v>158</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>2</v>
+        <v>159</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>3</v>
+        <v>160</v>
       </c>
     </row>
     <row r="2" spans="2:5" ht="16">
@@ -3453,37 +3474,43 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="B1:F71"/>
+  <dimension ref="B1:H71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="K40" sqref="K40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="5" width="26.33203125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="16.83203125" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="9" style="2"/>
+    <col min="1" max="7" width="26.33203125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="16.83203125" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="16">
+    <row r="1" spans="2:8" ht="16">
       <c r="B1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="6" t="s">
-        <v>2</v>
-      </c>
       <c r="E1" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="F1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="6" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="2" spans="2:6" ht="16">
+      <c r="G1" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="2:8" ht="16">
       <c r="B2" s="3" t="s">
         <v>108</v>
       </c>
@@ -3491,35 +3518,47 @@
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
-    </row>
-    <row r="3" spans="2:6" ht="32">
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+    </row>
+    <row r="3" spans="2:8" ht="32">
       <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
+      <c r="C3" s="3" t="s">
+        <v>106</v>
+      </c>
       <c r="D3" s="3"/>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="3"/>
+      <c r="F3" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="F3" s="3"/>
-    </row>
-    <row r="4" spans="2:6" ht="16">
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+    </row>
+    <row r="4" spans="2:8" ht="16">
       <c r="B4" s="3" t="s">
         <v>152</v>
       </c>
       <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
+      <c r="D4" s="3" t="s">
+        <v>5</v>
+      </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
-    </row>
-    <row r="5" spans="2:6" ht="16">
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+    </row>
+    <row r="5" spans="2:8" ht="16">
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
-      <c r="D5" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="E5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3" t="s">
+        <v>163</v>
+      </c>
       <c r="F5" s="3"/>
-    </row>
-    <row r="6" spans="2:6" ht="16">
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+    </row>
+    <row r="6" spans="2:8" ht="16">
       <c r="B6" s="3" t="s">
         <v>154</v>
       </c>
@@ -3527,8 +3566,10 @@
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
-    </row>
-    <row r="7" spans="2:6" ht="16">
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+    </row>
+    <row r="7" spans="2:8" ht="16">
       <c r="B7" s="3" t="s">
         <v>108</v>
       </c>
@@ -3536,44 +3577,54 @@
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
-    </row>
-    <row r="8" spans="2:6" ht="16">
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+    </row>
+    <row r="8" spans="2:8" ht="16">
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="3"/>
+      <c r="E8" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="E8" s="3"/>
       <c r="F8" s="3"/>
-    </row>
-    <row r="9" spans="2:6" ht="16">
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+    </row>
+    <row r="9" spans="2:8" ht="16">
       <c r="B9" s="3"/>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="3"/>
+      <c r="D9" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
-    </row>
-    <row r="10" spans="2:6" ht="16">
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+    </row>
+    <row r="10" spans="2:8" ht="16">
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="3"/>
+      <c r="E10" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="E10" s="3"/>
       <c r="F10" s="3"/>
-    </row>
-    <row r="11" spans="2:6" ht="32">
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+    </row>
+    <row r="11" spans="2:8" ht="32">
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
-      <c r="E11" s="3" t="s">
+      <c r="E11" s="3"/>
+      <c r="F11" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="F11" s="3"/>
-    </row>
-    <row r="12" spans="2:6" ht="16">
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+    </row>
+    <row r="12" spans="2:8" ht="16">
       <c r="B12" s="3" t="s">
         <v>145</v>
       </c>
@@ -3581,17 +3632,21 @@
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
-    </row>
-    <row r="13" spans="2:6" ht="32">
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+    </row>
+    <row r="13" spans="2:8" ht="32">
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="3"/>
+      <c r="E13" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="E13" s="3"/>
       <c r="F13" s="3"/>
-    </row>
-    <row r="14" spans="2:6" ht="16">
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+    </row>
+    <row r="14" spans="2:8" ht="16">
       <c r="B14" s="3" t="s">
         <v>147</v>
       </c>
@@ -3599,35 +3654,41 @@
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
-    </row>
-    <row r="15" spans="2:6" ht="16">
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+    </row>
+    <row r="15" spans="2:8" ht="16">
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
-      <c r="D15" s="3" t="s">
+      <c r="D15" s="3"/>
+      <c r="E15" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="E15" s="3"/>
       <c r="F15" s="3"/>
-    </row>
-    <row r="16" spans="2:6" ht="16">
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+    </row>
+    <row r="16" spans="2:8">
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
-      <c r="E16" s="3" t="s">
-        <v>5</v>
-      </c>
+      <c r="E16" s="3"/>
       <c r="F16" s="3"/>
-    </row>
-    <row r="17" spans="2:6" ht="16">
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+    </row>
+    <row r="17" spans="2:8" ht="16">
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
-      <c r="E17" s="3" t="s">
+      <c r="E17" s="3"/>
+      <c r="F17" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="F17" s="3"/>
-    </row>
-    <row r="18" spans="2:6" ht="16">
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+    </row>
+    <row r="18" spans="2:8" ht="16">
       <c r="B18" s="3" t="s">
         <v>109</v>
       </c>
@@ -3635,8 +3696,10 @@
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
-    </row>
-    <row r="19" spans="2:6" ht="16">
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+    </row>
+    <row r="19" spans="2:8" ht="16">
       <c r="B19" s="3" t="s">
         <v>132</v>
       </c>
@@ -3644,64 +3707,78 @@
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
-    </row>
-    <row r="20" spans="2:6" ht="16">
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+    </row>
+    <row r="20" spans="2:8" ht="16">
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
-      <c r="D20" s="3" t="s">
+      <c r="D20" s="3"/>
+      <c r="E20" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="E20" s="3"/>
       <c r="F20" s="3"/>
-    </row>
-    <row r="21" spans="2:6" ht="16">
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+    </row>
+    <row r="21" spans="2:8" ht="16">
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
-      <c r="E21" s="3" t="s">
+      <c r="E21" s="3"/>
+      <c r="F21" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="F21" s="3"/>
-    </row>
-    <row r="22" spans="2:6" ht="32">
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+    </row>
+    <row r="22" spans="2:8" ht="32">
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
-      <c r="F22" s="3" t="s">
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="23" spans="2:6" ht="16">
+    <row r="23" spans="2:8" ht="16">
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
-      <c r="E23" s="3" t="s">
+      <c r="E23" s="3"/>
+      <c r="F23" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="F23" s="3"/>
-    </row>
-    <row r="24" spans="2:6" ht="17">
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+    </row>
+    <row r="24" spans="2:8" ht="17">
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
-      <c r="D24" s="8" t="s">
+      <c r="D24" s="3"/>
+      <c r="E24" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="E24" s="8"/>
-      <c r="F24" s="8" t="s">
+      <c r="F24" s="8"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="8" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="25" spans="2:6" ht="16">
+    <row r="25" spans="2:8" ht="16">
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
-      <c r="E25" s="3" t="s">
+      <c r="E25" s="3"/>
+      <c r="F25" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="F25" s="3"/>
-    </row>
-    <row r="26" spans="2:6" ht="16">
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+    </row>
+    <row r="26" spans="2:8" ht="16">
       <c r="B26" s="3" t="s">
         <v>140</v>
       </c>
@@ -3709,17 +3786,21 @@
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
-    </row>
-    <row r="27" spans="2:6" ht="16">
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+    </row>
+    <row r="27" spans="2:8" ht="16">
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
-      <c r="D27" s="3" t="s">
+      <c r="D27" s="3"/>
+      <c r="E27" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="E27" s="3"/>
       <c r="F27" s="3"/>
-    </row>
-    <row r="28" spans="2:6" ht="16">
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+    </row>
+    <row r="28" spans="2:8" ht="16">
       <c r="B28" s="3" t="s">
         <v>109</v>
       </c>
@@ -3727,26 +3808,32 @@
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
-    </row>
-    <row r="29" spans="2:6" ht="16">
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+    </row>
+    <row r="29" spans="2:8" ht="16">
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
-      <c r="E29" s="3" t="s">
+      <c r="E29" s="3"/>
+      <c r="F29" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="F29" s="3"/>
-    </row>
-    <row r="30" spans="2:6" ht="16">
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+    </row>
+    <row r="30" spans="2:8" ht="16">
       <c r="B30" s="3"/>
-      <c r="C30" s="3" t="s">
+      <c r="C30" s="3"/>
+      <c r="D30" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="D30" s="3"/>
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
-    </row>
-    <row r="31" spans="2:6" ht="16">
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+    </row>
+    <row r="31" spans="2:8" ht="16">
       <c r="B31" s="3" t="s">
         <v>111</v>
       </c>
@@ -3754,35 +3841,43 @@
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
-    </row>
-    <row r="32" spans="2:6" ht="16">
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+    </row>
+    <row r="32" spans="2:8" ht="16">
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
-      <c r="D32" s="3" t="s">
+      <c r="D32" s="3"/>
+      <c r="E32" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="E32" s="3"/>
       <c r="F32" s="3"/>
-    </row>
-    <row r="33" spans="2:6" ht="16">
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
+    </row>
+    <row r="33" spans="2:8" ht="16">
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
-      <c r="E33" s="3" t="s">
+      <c r="E33" s="3"/>
+      <c r="F33" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="F33" s="3"/>
-    </row>
-    <row r="34" spans="2:6" ht="16">
+      <c r="G33" s="3"/>
+      <c r="H33" s="3"/>
+    </row>
+    <row r="34" spans="2:8" ht="16">
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
-      <c r="D34" s="3" t="s">
+      <c r="D34" s="3"/>
+      <c r="E34" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="E34" s="3"/>
       <c r="F34" s="3"/>
-    </row>
-    <row r="35" spans="2:6" ht="16">
+      <c r="G34" s="3"/>
+      <c r="H34" s="3"/>
+    </row>
+    <row r="35" spans="2:8" ht="16">
       <c r="B35" s="3" t="s">
         <v>114</v>
       </c>
@@ -3790,35 +3885,43 @@
       <c r="D35" s="3"/>
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
-    </row>
-    <row r="36" spans="2:6" ht="16">
+      <c r="G35" s="3"/>
+      <c r="H35" s="3"/>
+    </row>
+    <row r="36" spans="2:8" ht="16">
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
-      <c r="D36" s="3" t="s">
+      <c r="D36" s="3"/>
+      <c r="E36" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="E36" s="3"/>
       <c r="F36" s="3"/>
-    </row>
-    <row r="37" spans="2:6" ht="16">
+      <c r="G36" s="3"/>
+      <c r="H36" s="3"/>
+    </row>
+    <row r="37" spans="2:8" ht="16">
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
-      <c r="E37" s="3" t="s">
+      <c r="E37" s="3"/>
+      <c r="F37" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="F37" s="3"/>
-    </row>
-    <row r="38" spans="2:6" ht="16">
+      <c r="G37" s="3"/>
+      <c r="H37" s="3"/>
+    </row>
+    <row r="38" spans="2:8" ht="16">
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
-      <c r="D38" s="3" t="s">
+      <c r="D38" s="3"/>
+      <c r="E38" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="E38" s="3"/>
       <c r="F38" s="3"/>
-    </row>
-    <row r="39" spans="2:6" ht="16">
+      <c r="G38" s="3"/>
+      <c r="H38" s="3"/>
+    </row>
+    <row r="39" spans="2:8" ht="16">
       <c r="B39" s="3" t="s">
         <v>155</v>
       </c>
@@ -3826,232 +3929,298 @@
       <c r="D39" s="3"/>
       <c r="E39" s="3"/>
       <c r="F39" s="3"/>
-    </row>
-    <row r="40" spans="2:6" ht="16">
+      <c r="G39" s="3"/>
+      <c r="H39" s="3"/>
+    </row>
+    <row r="40" spans="2:8" ht="16">
       <c r="B40" s="3"/>
-      <c r="C40" s="4"/>
-      <c r="D40" s="3"/>
-      <c r="E40" s="3" t="s">
+      <c r="C40" s="3"/>
+      <c r="D40" s="4"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="F40" s="3"/>
-    </row>
-    <row r="41" spans="2:6">
+      <c r="G40" s="3"/>
+      <c r="H40" s="3"/>
+    </row>
+    <row r="41" spans="2:8">
       <c r="B41" s="3"/>
-      <c r="C41" s="4"/>
-      <c r="D41" s="3"/>
+      <c r="C41" s="3"/>
+      <c r="D41" s="4"/>
       <c r="E41" s="3"/>
       <c r="F41" s="3"/>
-    </row>
-    <row r="42" spans="2:6">
+      <c r="G41" s="3"/>
+      <c r="H41" s="3"/>
+    </row>
+    <row r="42" spans="2:8">
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
       <c r="E42" s="3"/>
       <c r="F42" s="3"/>
-    </row>
-    <row r="43" spans="2:6">
+      <c r="G42" s="3"/>
+      <c r="H42" s="3"/>
+    </row>
+    <row r="43" spans="2:8">
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
       <c r="E43" s="3"/>
       <c r="F43" s="3"/>
-    </row>
-    <row r="44" spans="2:6">
+      <c r="G43" s="3"/>
+      <c r="H43" s="3"/>
+    </row>
+    <row r="44" spans="2:8">
       <c r="B44" s="3"/>
-      <c r="C44" s="4"/>
-      <c r="D44" s="3"/>
+      <c r="C44" s="3"/>
+      <c r="D44" s="4"/>
       <c r="E44" s="3"/>
       <c r="F44" s="3"/>
-    </row>
-    <row r="45" spans="2:6">
+      <c r="G44" s="3"/>
+      <c r="H44" s="3"/>
+    </row>
+    <row r="45" spans="2:8">
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
       <c r="E45" s="3"/>
       <c r="F45" s="3"/>
-    </row>
-    <row r="46" spans="2:6">
+      <c r="G45" s="3"/>
+      <c r="H45" s="3"/>
+    </row>
+    <row r="46" spans="2:8">
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
       <c r="E46" s="3"/>
       <c r="F46" s="3"/>
-    </row>
-    <row r="47" spans="2:6">
+      <c r="G46" s="3"/>
+      <c r="H46" s="3"/>
+    </row>
+    <row r="47" spans="2:8">
       <c r="B47" s="3"/>
-      <c r="C47" s="4"/>
-      <c r="D47" s="3"/>
+      <c r="C47" s="3"/>
+      <c r="D47" s="4"/>
       <c r="E47" s="3"/>
       <c r="F47" s="3"/>
-    </row>
-    <row r="48" spans="2:6">
+      <c r="G47" s="3"/>
+      <c r="H47" s="3"/>
+    </row>
+    <row r="48" spans="2:8">
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
       <c r="D48" s="3"/>
       <c r="E48" s="3"/>
       <c r="F48" s="3"/>
-    </row>
-    <row r="49" spans="2:6">
+      <c r="G48" s="3"/>
+      <c r="H48" s="3"/>
+    </row>
+    <row r="49" spans="2:8">
       <c r="B49" s="4"/>
-      <c r="C49" s="3"/>
+      <c r="C49" s="4"/>
       <c r="D49" s="3"/>
       <c r="E49" s="3"/>
       <c r="F49" s="3"/>
-    </row>
-    <row r="50" spans="2:6">
+      <c r="G49" s="3"/>
+      <c r="H49" s="3"/>
+    </row>
+    <row r="50" spans="2:8">
       <c r="B50" s="3"/>
       <c r="C50" s="3"/>
       <c r="D50" s="3"/>
       <c r="E50" s="3"/>
       <c r="F50" s="3"/>
-    </row>
-    <row r="51" spans="2:6">
+      <c r="G50" s="3"/>
+      <c r="H50" s="3"/>
+    </row>
+    <row r="51" spans="2:8">
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
       <c r="D51" s="3"/>
       <c r="E51" s="3"/>
       <c r="F51" s="3"/>
-    </row>
-    <row r="52" spans="2:6">
+      <c r="G51" s="3"/>
+      <c r="H51" s="3"/>
+    </row>
+    <row r="52" spans="2:8">
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
       <c r="D52" s="3"/>
       <c r="E52" s="3"/>
       <c r="F52" s="3"/>
-    </row>
-    <row r="53" spans="2:6">
+      <c r="G52" s="3"/>
+      <c r="H52" s="3"/>
+    </row>
+    <row r="53" spans="2:8">
       <c r="B53" s="3"/>
-      <c r="C53" s="4"/>
-      <c r="D53" s="3"/>
+      <c r="C53" s="3"/>
+      <c r="D53" s="4"/>
       <c r="E53" s="3"/>
       <c r="F53" s="3"/>
-    </row>
-    <row r="54" spans="2:6">
+      <c r="G53" s="3"/>
+      <c r="H53" s="3"/>
+    </row>
+    <row r="54" spans="2:8">
       <c r="B54" s="3"/>
       <c r="C54" s="3"/>
       <c r="D54" s="3"/>
       <c r="E54" s="3"/>
       <c r="F54" s="3"/>
-    </row>
-    <row r="55" spans="2:6">
+      <c r="G54" s="3"/>
+      <c r="H54" s="3"/>
+    </row>
+    <row r="55" spans="2:8">
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
       <c r="D55" s="3"/>
       <c r="E55" s="3"/>
       <c r="F55" s="3"/>
-    </row>
-    <row r="56" spans="2:6">
+      <c r="G55" s="3"/>
+      <c r="H55" s="3"/>
+    </row>
+    <row r="56" spans="2:8">
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>
       <c r="D56" s="3"/>
       <c r="E56" s="3"/>
       <c r="F56" s="3"/>
-    </row>
-    <row r="57" spans="2:6">
+      <c r="G56" s="3"/>
+      <c r="H56" s="3"/>
+    </row>
+    <row r="57" spans="2:8">
       <c r="B57" s="3"/>
       <c r="C57" s="3"/>
       <c r="D57" s="3"/>
       <c r="E57" s="3"/>
       <c r="F57" s="3"/>
-    </row>
-    <row r="58" spans="2:6">
+      <c r="G57" s="3"/>
+      <c r="H57" s="3"/>
+    </row>
+    <row r="58" spans="2:8">
       <c r="B58" s="3"/>
-      <c r="C58" s="4"/>
-      <c r="D58" s="3"/>
+      <c r="C58" s="3"/>
+      <c r="D58" s="4"/>
       <c r="E58" s="3"/>
       <c r="F58" s="3"/>
-    </row>
-    <row r="59" spans="2:6">
+      <c r="G58" s="3"/>
+      <c r="H58" s="3"/>
+    </row>
+    <row r="59" spans="2:8">
       <c r="B59" s="3"/>
       <c r="C59" s="3"/>
       <c r="D59" s="3"/>
       <c r="E59" s="3"/>
       <c r="F59" s="3"/>
-    </row>
-    <row r="60" spans="2:6">
+      <c r="G59" s="3"/>
+      <c r="H59" s="3"/>
+    </row>
+    <row r="60" spans="2:8">
       <c r="B60" s="3"/>
       <c r="C60" s="3"/>
       <c r="D60" s="3"/>
       <c r="E60" s="3"/>
       <c r="F60" s="3"/>
-    </row>
-    <row r="61" spans="2:6">
+      <c r="G60" s="3"/>
+      <c r="H60" s="3"/>
+    </row>
+    <row r="61" spans="2:8">
       <c r="B61" s="3"/>
       <c r="C61" s="3"/>
       <c r="D61" s="3"/>
       <c r="E61" s="3"/>
       <c r="F61" s="3"/>
-    </row>
-    <row r="62" spans="2:6">
+      <c r="G61" s="3"/>
+      <c r="H61" s="3"/>
+    </row>
+    <row r="62" spans="2:8">
       <c r="B62" s="3"/>
       <c r="C62" s="3"/>
       <c r="D62" s="3"/>
       <c r="E62" s="3"/>
       <c r="F62" s="3"/>
-    </row>
-    <row r="63" spans="2:6">
+      <c r="G62" s="3"/>
+      <c r="H62" s="3"/>
+    </row>
+    <row r="63" spans="2:8">
       <c r="B63" s="3"/>
       <c r="C63" s="3"/>
       <c r="D63" s="3"/>
       <c r="E63" s="3"/>
       <c r="F63" s="3"/>
-    </row>
-    <row r="64" spans="2:6">
+      <c r="G63" s="3"/>
+      <c r="H63" s="3"/>
+    </row>
+    <row r="64" spans="2:8">
       <c r="B64" s="3"/>
       <c r="C64" s="3"/>
       <c r="D64" s="3"/>
       <c r="E64" s="3"/>
       <c r="F64" s="3"/>
-    </row>
-    <row r="65" spans="2:6">
+      <c r="G64" s="3"/>
+      <c r="H64" s="3"/>
+    </row>
+    <row r="65" spans="2:8">
       <c r="B65" s="3"/>
-      <c r="C65" s="4"/>
-      <c r="D65" s="3"/>
+      <c r="C65" s="3"/>
+      <c r="D65" s="4"/>
       <c r="E65" s="3"/>
       <c r="F65" s="3"/>
-    </row>
-    <row r="66" spans="2:6">
+      <c r="G65" s="3"/>
+      <c r="H65" s="3"/>
+    </row>
+    <row r="66" spans="2:8">
       <c r="B66" s="3"/>
       <c r="C66" s="3"/>
       <c r="D66" s="3"/>
       <c r="E66" s="3"/>
       <c r="F66" s="3"/>
-    </row>
-    <row r="67" spans="2:6">
+      <c r="G66" s="3"/>
+      <c r="H66" s="3"/>
+    </row>
+    <row r="67" spans="2:8">
       <c r="B67" s="3"/>
       <c r="C67" s="3"/>
       <c r="D67" s="3"/>
       <c r="E67" s="3"/>
       <c r="F67" s="3"/>
-    </row>
-    <row r="68" spans="2:6">
+      <c r="G67" s="3"/>
+      <c r="H67" s="3"/>
+    </row>
+    <row r="68" spans="2:8">
       <c r="B68" s="3"/>
-      <c r="C68" s="4"/>
-      <c r="D68" s="3"/>
+      <c r="C68" s="3"/>
+      <c r="D68" s="4"/>
       <c r="E68" s="3"/>
       <c r="F68" s="3"/>
-    </row>
-    <row r="69" spans="2:6">
+      <c r="G68" s="3"/>
+      <c r="H68" s="3"/>
+    </row>
+    <row r="69" spans="2:8">
       <c r="B69" s="3"/>
       <c r="C69" s="3"/>
       <c r="D69" s="3"/>
       <c r="E69" s="3"/>
       <c r="F69" s="3"/>
-    </row>
-    <row r="70" spans="2:6">
+      <c r="G69" s="3"/>
+      <c r="H69" s="3"/>
+    </row>
+    <row r="70" spans="2:8">
       <c r="B70" s="3"/>
       <c r="C70" s="3"/>
       <c r="D70" s="3"/>
       <c r="E70" s="3"/>
       <c r="F70" s="3"/>
-    </row>
-    <row r="71" spans="2:6">
+      <c r="G70" s="3"/>
+      <c r="H70" s="3"/>
+    </row>
+    <row r="71" spans="2:8">
       <c r="B71" s="3"/>
       <c r="C71" s="3"/>
       <c r="D71" s="3"/>
       <c r="E71" s="3"/>
       <c r="F71" s="3"/>
+      <c r="G71" s="3"/>
+      <c r="H71" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>